<commit_message>
Add final project report PDF and update .py
</commit_message>
<xml_diff>
--- a/data/processed/processed_macro_correlation.xlsx
+++ b/data/processed/processed_macro_correlation.xlsx
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.6093578524970937</v>
+        <v>0.6093030477783118</v>
       </c>
     </row>
     <row r="8">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1024092795006399</v>
+        <v>0.1012514823897827</v>
       </c>
     </row>
     <row r="10">

</xml_diff>